<commit_message>
Updated Whitepaper and Website with new Team
</commit_message>
<xml_diff>
--- a/Positions.xlsx
+++ b/Positions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Onasander\GitHub\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7464A852-50CF-43C4-BA18-BE4B8E8AD799}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{760AD338-4816-4E30-AF06-2C888E337040}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8EEF8E4D-6163-4A57-9F1C-58B1E69BBC64}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Jr. Business Analyst</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>aw88techsoft</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/robert-muer-b97742165/</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,6 +943,9 @@
     <row r="47" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">

</xml_diff>